<commit_message>
Colorcoded attributes file, update to first data plot
</commit_message>
<xml_diff>
--- a/data/ruimtelijke_kengetallen2019/verklaringattributenruimtelijkekengetallen2019.xlsx
+++ b/data/ruimtelijke_kengetallen2019/verklaringattributenruimtelijkekengetallen2019.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\GitKraken\OpenDataDenHaag\data\ruimtelijke_kengetallen2019\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5AE403D-3D28-4A3C-B843-D493DF466A40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="315" windowWidth="24540" windowHeight="10680"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ruimtelijkekengetallen2019" sheetId="1" r:id="rId1"/>
@@ -610,7 +616,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -628,12 +634,54 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -648,9 +696,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -661,6 +716,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -668,7 +726,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -706,9 +764,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -741,9 +799,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -776,9 +851,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -951,11 +1043,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="J78" sqref="J78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1141,122 +1233,122 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E16">
-        <v>2019</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="E16" s="2">
+        <v>2019</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E17">
-        <v>2019</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="E17" s="2">
+        <v>2019</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="C18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E18">
-        <v>2019</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="E18" s="2">
+        <v>2019</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E19">
-        <v>2019</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="E19" s="2">
+        <v>2019</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="C20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E20">
-        <v>2019</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="E20" s="2">
+        <v>2019</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="C21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E21">
-        <v>2019</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="E21" s="2">
+        <v>2019</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1281,22 +1373,22 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="C23" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="E23">
-        <v>2019</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="E23" s="3">
+        <v>2019</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1441,442 +1533,442 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C31" t="s">
-        <v>34</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="C31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E31">
-        <v>2019</v>
-      </c>
-      <c r="F31" t="s">
+      <c r="E31" s="2">
+        <v>2019</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C32" t="s">
-        <v>34</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="C32" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E32">
-        <v>2019</v>
-      </c>
-      <c r="F32" t="s">
+      <c r="E32" s="2">
+        <v>2019</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C33" t="s">
-        <v>34</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="C33" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E33">
-        <v>2019</v>
-      </c>
-      <c r="F33" t="s">
+      <c r="E33" s="2">
+        <v>2019</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C34" t="s">
-        <v>34</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="C34" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E34">
-        <v>2019</v>
-      </c>
-      <c r="F34" t="s">
+      <c r="E34" s="2">
+        <v>2019</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C35" t="s">
-        <v>34</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="C35" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E35">
-        <v>2019</v>
-      </c>
-      <c r="F35" t="s">
+      <c r="E35" s="2">
+        <v>2019</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C36" t="s">
-        <v>34</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="C36" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E36">
-        <v>2019</v>
-      </c>
-      <c r="F36" t="s">
+      <c r="E36" s="4">
+        <v>2019</v>
+      </c>
+      <c r="F36" s="4" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C37" t="s">
-        <v>34</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="C37" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D37" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E37">
-        <v>2019</v>
-      </c>
-      <c r="F37" t="s">
+      <c r="E37" s="4">
+        <v>2019</v>
+      </c>
+      <c r="F37" s="4" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C38" t="s">
-        <v>34</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="C38" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E38">
-        <v>2019</v>
-      </c>
-      <c r="F38" t="s">
+      <c r="E38" s="4">
+        <v>2019</v>
+      </c>
+      <c r="F38" s="4" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C39" t="s">
-        <v>34</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="C39" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E39">
-        <v>2019</v>
-      </c>
-      <c r="F39" t="s">
+      <c r="E39" s="4">
+        <v>2019</v>
+      </c>
+      <c r="F39" s="4" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="C40" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E40">
-        <v>2019</v>
-      </c>
-      <c r="F40" t="s">
+      <c r="E40" s="4">
+        <v>2019</v>
+      </c>
+      <c r="F40" s="4" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C41" t="s">
-        <v>34</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="C41" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E41">
-        <v>2019</v>
-      </c>
-      <c r="F41" t="s">
+      <c r="E41" s="4">
+        <v>2019</v>
+      </c>
+      <c r="F41" s="4" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="A42" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C42" t="s">
-        <v>34</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="C42" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E42">
-        <v>2019</v>
-      </c>
-      <c r="F42" t="s">
+      <c r="E42" s="4">
+        <v>2019</v>
+      </c>
+      <c r="F42" s="4" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="A43" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C43" t="s">
-        <v>34</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="C43" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E43">
-        <v>2019</v>
-      </c>
-      <c r="F43" t="s">
+      <c r="E43" s="4">
+        <v>2019</v>
+      </c>
+      <c r="F43" s="4" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A44" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C44" t="s">
-        <v>34</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="C44" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D44" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="E44">
-        <v>2019</v>
-      </c>
-      <c r="F44" t="s">
+      <c r="E44" s="4">
+        <v>2019</v>
+      </c>
+      <c r="F44" s="4" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="A45" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C45" t="s">
-        <v>34</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="C45" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D45" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E45">
-        <v>2019</v>
-      </c>
-      <c r="F45" t="s">
+      <c r="E45" s="4">
+        <v>2019</v>
+      </c>
+      <c r="F45" s="4" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="A46" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C46" t="s">
-        <v>34</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="C46" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D46" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="E46">
-        <v>2019</v>
-      </c>
-      <c r="F46" t="s">
+      <c r="E46" s="4">
+        <v>2019</v>
+      </c>
+      <c r="F46" s="4" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="A47" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C47" t="s">
-        <v>34</v>
-      </c>
-      <c r="D47" t="s">
+      <c r="C47" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D47" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E47">
-        <v>2019</v>
-      </c>
-      <c r="F47" t="s">
+      <c r="E47" s="4">
+        <v>2019</v>
+      </c>
+      <c r="F47" s="4" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="A48" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C48" t="s">
-        <v>34</v>
-      </c>
-      <c r="D48" t="s">
+      <c r="C48" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D48" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="E48">
-        <v>2019</v>
-      </c>
-      <c r="F48" t="s">
+      <c r="E48" s="4">
+        <v>2019</v>
+      </c>
+      <c r="F48" s="4" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="A49" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C49" t="s">
-        <v>34</v>
-      </c>
-      <c r="D49" t="s">
+      <c r="C49" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D49" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="E49">
-        <v>2019</v>
-      </c>
-      <c r="F49" t="s">
+      <c r="E49" s="5">
+        <v>2019</v>
+      </c>
+      <c r="F49" s="5" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="A50" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C50" t="s">
-        <v>34</v>
-      </c>
-      <c r="D50" t="s">
+      <c r="C50" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D50" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E50">
-        <v>2019</v>
-      </c>
-      <c r="F50" t="s">
+      <c r="E50" s="5">
+        <v>2019</v>
+      </c>
+      <c r="F50" s="5" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="A51" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C51" t="s">
-        <v>34</v>
-      </c>
-      <c r="D51" t="s">
+      <c r="C51" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D51" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="E51">
-        <v>2019</v>
-      </c>
-      <c r="F51" t="s">
+      <c r="E51" s="5">
+        <v>2019</v>
+      </c>
+      <c r="F51" s="5" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="A52" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C52" t="s">
-        <v>34</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="C52" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D52" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="E52">
-        <v>2019</v>
-      </c>
-      <c r="F52" t="s">
+      <c r="E52" s="5">
+        <v>2019</v>
+      </c>
+      <c r="F52" s="5" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1921,22 +2013,22 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="A55" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C55" t="s">
-        <v>34</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="C55" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D55" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="E55">
-        <v>2019</v>
-      </c>
-      <c r="F55" t="s">
+      <c r="E55" s="6">
+        <v>2019</v>
+      </c>
+      <c r="F55" s="6" t="s">
         <v>123</v>
       </c>
     </row>
@@ -1981,302 +2073,302 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="A58" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C58" t="s">
-        <v>34</v>
-      </c>
-      <c r="D58" t="s">
+      <c r="C58" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D58" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="E58">
-        <v>2019</v>
-      </c>
-      <c r="F58" t="s">
+      <c r="E58" s="7">
+        <v>2019</v>
+      </c>
+      <c r="F58" s="7" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="A59" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C59" t="s">
-        <v>34</v>
-      </c>
-      <c r="D59" t="s">
+      <c r="C59" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D59" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="E59">
-        <v>2019</v>
-      </c>
-      <c r="F59" t="s">
+      <c r="E59" s="7">
+        <v>2019</v>
+      </c>
+      <c r="F59" s="7" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="A60" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C60" t="s">
-        <v>34</v>
-      </c>
-      <c r="D60" t="s">
+      <c r="C60" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D60" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="E60">
-        <v>2019</v>
-      </c>
-      <c r="F60" t="s">
+      <c r="E60" s="7">
+        <v>2019</v>
+      </c>
+      <c r="F60" s="7" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="A61" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C61" t="s">
-        <v>34</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="C61" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D61" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="E61">
-        <v>2019</v>
-      </c>
-      <c r="F61" t="s">
+      <c r="E61" s="7">
+        <v>2019</v>
+      </c>
+      <c r="F61" s="7" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="A62" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C62" t="s">
-        <v>34</v>
-      </c>
-      <c r="D62" t="s">
+      <c r="C62" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D62" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="E62">
-        <v>2019</v>
-      </c>
-      <c r="F62" t="s">
+      <c r="E62" s="7">
+        <v>2019</v>
+      </c>
+      <c r="F62" s="7" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="A63" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C63" t="s">
-        <v>34</v>
-      </c>
-      <c r="D63" t="s">
+      <c r="C63" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D63" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="E63">
-        <v>2019</v>
-      </c>
-      <c r="F63" t="s">
+      <c r="E63" s="7">
+        <v>2019</v>
+      </c>
+      <c r="F63" s="7" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="A64" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C64" t="s">
-        <v>34</v>
-      </c>
-      <c r="D64" t="s">
+      <c r="C64" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D64" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E64">
-        <v>2019</v>
-      </c>
-      <c r="F64" t="s">
+      <c r="E64" s="7">
+        <v>2019</v>
+      </c>
+      <c r="F64" s="7" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="A65" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C65" t="s">
-        <v>34</v>
-      </c>
-      <c r="D65" t="s">
+      <c r="C65" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D65" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="E65">
-        <v>2019</v>
-      </c>
-      <c r="F65" t="s">
+      <c r="E65" s="7">
+        <v>2019</v>
+      </c>
+      <c r="F65" s="7" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="A66" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C66" t="s">
-        <v>34</v>
-      </c>
-      <c r="D66" t="s">
+      <c r="C66" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D66" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="E66">
-        <v>2019</v>
-      </c>
-      <c r="F66" t="s">
+      <c r="E66" s="7">
+        <v>2019</v>
+      </c>
+      <c r="F66" s="7" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="A67" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C67" t="s">
-        <v>34</v>
-      </c>
-      <c r="D67" t="s">
+      <c r="C67" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D67" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="E67">
-        <v>2019</v>
-      </c>
-      <c r="F67" t="s">
+      <c r="E67" s="7">
+        <v>2019</v>
+      </c>
+      <c r="F67" s="7" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="A68" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C68" t="s">
-        <v>34</v>
-      </c>
-      <c r="D68" t="s">
+      <c r="C68" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D68" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="E68">
-        <v>2019</v>
-      </c>
-      <c r="F68" t="s">
+      <c r="E68" s="7">
+        <v>2019</v>
+      </c>
+      <c r="F68" s="7" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="A69" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C69" t="s">
-        <v>34</v>
-      </c>
-      <c r="D69" t="s">
+      <c r="C69" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D69" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="E69">
-        <v>2019</v>
-      </c>
-      <c r="F69" t="s">
+      <c r="E69" s="7">
+        <v>2019</v>
+      </c>
+      <c r="F69" s="7" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="A70" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C70" t="s">
-        <v>34</v>
-      </c>
-      <c r="D70" t="s">
+      <c r="C70" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D70" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="E70">
-        <v>2019</v>
-      </c>
-      <c r="F70" t="s">
+      <c r="E70" s="7">
+        <v>2019</v>
+      </c>
+      <c r="F70" s="7" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="A71" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C71" t="s">
-        <v>34</v>
-      </c>
-      <c r="D71" t="s">
+      <c r="C71" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D71" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="E71">
-        <v>2019</v>
-      </c>
-      <c r="F71" t="s">
+      <c r="E71" s="7">
+        <v>2019</v>
+      </c>
+      <c r="F71" s="7" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="A72" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C72" t="s">
-        <v>34</v>
-      </c>
-      <c r="D72" t="s">
+      <c r="C72" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D72" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="E72">
-        <v>2019</v>
-      </c>
-      <c r="F72" t="s">
+      <c r="E72" s="7">
+        <v>2019</v>
+      </c>
+      <c r="F72" s="7" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2301,22 +2393,22 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="A74" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C74" t="s">
-        <v>34</v>
-      </c>
-      <c r="D74" t="s">
+      <c r="C74" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D74" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E74">
-        <v>2019</v>
-      </c>
-      <c r="F74" t="s">
+      <c r="E74" s="2">
+        <v>2019</v>
+      </c>
+      <c r="F74" s="2" t="s">
         <v>162</v>
       </c>
     </row>
@@ -2341,22 +2433,22 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="A76" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C76" t="s">
-        <v>34</v>
-      </c>
-      <c r="D76" t="s">
+      <c r="C76" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D76" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="E76">
+      <c r="E76" s="2">
         <v>2017</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F76" s="2" t="s">
         <v>170</v>
       </c>
     </row>
@@ -2541,42 +2633,42 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+      <c r="A86" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="C86" t="s">
-        <v>34</v>
-      </c>
-      <c r="D86" t="s">
+      <c r="C86" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D86" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="E86">
-        <v>2019</v>
-      </c>
-      <c r="F86" t="s">
+      <c r="E86" s="8">
+        <v>2019</v>
+      </c>
+      <c r="F86" s="8" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+      <c r="A87" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="C87" t="s">
-        <v>34</v>
-      </c>
-      <c r="D87" t="s">
+      <c r="C87" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D87" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="E87">
-        <v>2019</v>
-      </c>
-      <c r="F87" t="s">
+      <c r="E87" s="8">
+        <v>2019</v>
+      </c>
+      <c r="F87" s="8" t="s">
         <v>192</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New data sources, some new calculations
</commit_message>
<xml_diff>
--- a/data/ruimtelijke_kengetallen2019/verklaringattributenruimtelijkekengetallen2019.xlsx
+++ b/data/ruimtelijke_kengetallen2019/verklaringattributenruimtelijkekengetallen2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\GitKraken\OpenDataDenHaag\data\ruimtelijke_kengetallen2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5AE403D-3D28-4A3C-B843-D493DF466A40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5CA1364-8E75-418B-A94D-C3BFDDE26249}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -634,7 +634,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -679,7 +679,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -696,7 +702,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -706,6 +712,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1046,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="J78" sqref="J78"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K74" sqref="K74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1353,22 +1361,22 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C22" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="C22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E22">
-        <v>2019</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="E22" s="3">
+        <v>2019</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1393,42 +1401,42 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C24" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="C24" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="E24">
-        <v>2019</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="E24" s="10">
+        <v>2019</v>
+      </c>
+      <c r="F24" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C25" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="C25" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="10">
         <v>2018</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="10" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1973,22 +1981,22 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="A53" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C53" t="s">
-        <v>34</v>
-      </c>
-      <c r="D53" t="s">
+      <c r="C53" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D53" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="E53">
-        <v>2019</v>
-      </c>
-      <c r="F53" t="s">
+      <c r="E53" s="8">
+        <v>2019</v>
+      </c>
+      <c r="F53" s="8" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2633,42 +2641,42 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="8" t="s">
+      <c r="A86" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="B86" s="8" t="s">
+      <c r="B86" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="C86" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D86" s="8" t="s">
+      <c r="C86" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D86" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="E86" s="8">
-        <v>2019</v>
-      </c>
-      <c r="F86" s="8" t="s">
+      <c r="E86" s="9">
+        <v>2019</v>
+      </c>
+      <c r="F86" s="9" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="8" t="s">
+      <c r="A87" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="B87" s="8" t="s">
+      <c r="B87" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="C87" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D87" s="8" t="s">
+      <c r="C87" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D87" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="E87" s="8">
-        <v>2019</v>
-      </c>
-      <c r="F87" s="8" t="s">
+      <c r="E87" s="9">
+        <v>2019</v>
+      </c>
+      <c r="F87" s="9" t="s">
         <v>192</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Slight changes to selected variables for model use
</commit_message>
<xml_diff>
--- a/data/ruimtelijke_kengetallen2019/verklaringattributenruimtelijkekengetallen2019.xlsx
+++ b/data/ruimtelijke_kengetallen2019/verklaringattributenruimtelijkekengetallen2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\GitKraken\OpenDataDenHaag\data\ruimtelijke_kengetallen2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5CA1364-8E75-418B-A94D-C3BFDDE26249}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660E5624-636C-4354-A0D1-8ADFB914A49B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1054,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K74" sqref="K74"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="K68" sqref="K68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2101,22 +2101,22 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="7" t="s">
+      <c r="A59" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B59" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="C59" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D59" s="7" t="s">
+      <c r="C59" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D59" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="E59" s="7">
-        <v>2019</v>
-      </c>
-      <c r="F59" s="7" t="s">
+      <c r="E59" s="9">
+        <v>2019</v>
+      </c>
+      <c r="F59" s="9" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2141,82 +2141,82 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="7" t="s">
+      <c r="A61" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B61" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="C61" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D61" s="7" t="s">
+      <c r="C61" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D61" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="E61" s="7">
-        <v>2019</v>
-      </c>
-      <c r="F61" s="7" t="s">
+      <c r="E61" s="9">
+        <v>2019</v>
+      </c>
+      <c r="F61" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="7" t="s">
+      <c r="A62" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="B62" s="7" t="s">
+      <c r="B62" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="C62" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D62" s="7" t="s">
+      <c r="C62" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D62" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="E62" s="7">
-        <v>2019</v>
-      </c>
-      <c r="F62" s="7" t="s">
+      <c r="E62" s="9">
+        <v>2019</v>
+      </c>
+      <c r="F62" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="7" t="s">
+      <c r="A63" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="B63" s="7" t="s">
+      <c r="B63" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="C63" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D63" s="7" t="s">
+      <c r="C63" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D63" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="E63" s="7">
-        <v>2019</v>
-      </c>
-      <c r="F63" s="7" t="s">
+      <c r="E63" s="9">
+        <v>2019</v>
+      </c>
+      <c r="F63" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
+      <c r="A64" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="B64" s="7" t="s">
+      <c r="B64" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="C64" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D64" s="7" t="s">
+      <c r="C64" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D64" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="E64" s="7">
-        <v>2019</v>
-      </c>
-      <c r="F64" s="7" t="s">
+      <c r="E64" s="9">
+        <v>2019</v>
+      </c>
+      <c r="F64" s="9" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2341,42 +2341,42 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="7" t="s">
+      <c r="A71" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="B71" s="7" t="s">
+      <c r="B71" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="C71" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D71" s="7" t="s">
+      <c r="C71" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D71" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="E71" s="7">
-        <v>2019</v>
-      </c>
-      <c r="F71" s="7" t="s">
+      <c r="E71" s="9">
+        <v>2019</v>
+      </c>
+      <c r="F71" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="7" t="s">
+      <c r="A72" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="B72" s="7" t="s">
+      <c r="B72" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="C72" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D72" s="7" t="s">
+      <c r="C72" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D72" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="E72" s="7">
-        <v>2019</v>
-      </c>
-      <c r="F72" s="7" t="s">
+      <c r="E72" s="9">
+        <v>2019</v>
+      </c>
+      <c r="F72" s="9" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>